<commit_message>
Added high costs in matrix to bandaid problem.
</commit_message>
<xml_diff>
--- a/Washington_New.xlsx
+++ b/Washington_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\MATLAB\ModelingandConsulting\Proj3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6111657F-CE1B-4A4F-A4F9-CD660E3381A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC64E54-D397-44A9-95CC-6B9A2060B90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="3" xr2:uid="{51C58A30-D6B0-4ACF-B549-DFDC5E34590D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="13" xr2:uid="{51C58A30-D6B0-4ACF-B549-DFDC5E34590D}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFE9D0-F344-49E1-BCD8-D293D9D4B06D}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="B2:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,7 +1276,7 @@
         <v>82</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>150000</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,7 +1689,7 @@
         <v>8</v>
       </c>
       <c r="H8">
-        <v>8</v>
+        <v>150000</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1941,7 +1941,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,7 +1965,7 @@
         <v>119</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>150000</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2005,7 +2005,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>150000</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3112,7 +3112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB059037-0953-44F1-B52A-F75E759EAC2B}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>